<commit_message>
Cambio de graficos seccion brechas de ingresos. Sacamos valuacion por tipo de ingreso. Arreglo del calculo ponderadores provincias, y texto Sin desc Jub.
</commit_message>
<xml_diff>
--- a/www/metadata.xlsx
+++ b/www/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\carol\Documents\Ecofeminita-general\shinyapp\www\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\ECOFEMINITA\shinyapp\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EE1604-2868-4D64-9851-C1A27B326957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDF54B6-819C-49B3-A071-B0BF19D35913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -123,9 +123,6 @@
     <t>B-Ingreso horario de la Ocupación Principal</t>
   </si>
   <si>
-    <t>B-Ingreso de la Ocupación Principal - Asalariadas/os sin desc. Jubil</t>
-  </si>
-  <si>
     <t>Desagregación edad</t>
   </si>
   <si>
@@ -264,10 +261,13 @@
     <t>La "brecha de ingreso horario de la ocupación principal" calcula la diferencia entre los ingresos por hora promedio percibidos por el empleo principal de los varones y las mujeres, expresada en términos del promedio percibido por los varones (generalmente el más alto). Es decir, que puede leerse como “por cada hora que trabajan en su ocupación principal, las mujeres perciben un ingreso, en promedio, …% menos que los de los varones”. Nos interesa estudiar la desigualdad en los ingresos en el pago por hora, teniendo en cuenta que la cantidad de tiempo destinado al mercado productivo no es igual entre varones y mujeres, porque son ellas quienes trabajan menos horas remuneradas para destinar tiempo al trabajo no pago del hogar y cuidados.</t>
   </si>
   <si>
-    <t>Lo que se conoce como "brecha salarial" calcula la diferencia entre los salarios promedios percibidos por el empleo principal de los varones y las mujeres y la expresa en términos del promedio percibido por los varones (generalmente el más alto). Es decir, que puede leerse como “las mujeres perciben ingresos derivados de su ocupación principal que, en promedio, son un …% menores que los de los varones”. Nos interesa ver cómo se amplía esta diferencia para el caso de las personas que trabajan en el mercado informal porque las mujeres tienden a insertarse en mayor medida bajo esa condición, como el caso de la rama del servicio doméstico.</t>
-  </si>
-  <si>
     <t>Las responsabilidades de limpieza, cocina y gestión del hogar toman tiempo y son un trabajo invisibilizado. Este indicador busca visibilizar el género de la principal persona encargada de resolverlas en cada hogar. Los hogares de un único miembro se incluyen en el cómputo, y se excluyen los casos en que estas tareas son realizadas por una trabajadora de casas particulares. </t>
+  </si>
+  <si>
+    <t>B-Ingreso de la Ocupación Principal - Asalariadas/os sin desc. jubil</t>
+  </si>
+  <si>
+    <t>Identificar a quienes no cuentan con descuento jubilatorio es una forma de estimar la informalidad. La "brecha de ingreso de la ocupación principal para asalariadas/os sin descuento jubilatorio" calcula la diferencia entre los ingresos percibidos por el empleo principal de varones y mujeres "informales". La brecha se expresa en términos del promedio percibido por los varones (generalmente el más alto). Es decir, que puede leerse como “por cada hora que trabajan en su ocupación principal, las mujeres sin descuento jubilatorio perciben un ingreso, en promedio, …% menos que los varones sin descuento jubilatorio”.</t>
   </si>
 </sst>
 </file>
@@ -682,18 +682,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="53.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.77734375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="110.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="110.54296875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -704,345 +704,345 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="116" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="174" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="145" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="116" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="10" t="s">
+    </row>
+    <row r="28" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="9" t="s">
+      <c r="C28" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B29" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C29" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A31" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="10" t="s">
+      <c r="B33" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+      <c r="B34" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>